<commit_message>
Adding graph drawing to OLED
</commit_message>
<xml_diff>
--- a/Assets/Screens.xlsx
+++ b/Assets/Screens.xlsx
@@ -98,7 +98,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,6 +108,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -204,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="255"/>
@@ -230,6 +236,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1260,7 +1270,7 @@
   <dimension ref="A1:DZ65"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="AY36" sqref="AY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4199,7 +4209,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DY65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="BY17" sqref="BY17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4493,7 +4508,7 @@
       <c r="CR1" s="1">
         <v>94</v>
       </c>
-      <c r="CS1" s="1">
+      <c r="CS1" s="23">
         <v>95</v>
       </c>
       <c r="CT1" s="1">
@@ -4589,7 +4604,7 @@
       <c r="DX1" s="1">
         <v>126</v>
       </c>
-      <c r="DY1" s="1">
+      <c r="DY1" s="23">
         <v>127</v>
       </c>
     </row>
@@ -6156,7 +6171,7 @@
       <c r="CH16" s="22"/>
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="24">
         <v>15</v>
       </c>
       <c r="B17" s="17"/>
@@ -8272,7 +8287,7 @@
       <c r="DY32" s="22"/>
     </row>
     <row r="33" spans="1:129" x14ac:dyDescent="0.25">
-      <c r="A33" s="20">
+      <c r="A33" s="24">
         <v>31</v>
       </c>
       <c r="B33" s="17"/>
@@ -12412,7 +12427,7 @@
       <c r="DY64" s="22"/>
     </row>
     <row r="65" spans="1:129" x14ac:dyDescent="0.25">
-      <c r="A65" s="20">
+      <c r="A65" s="24">
         <v>63</v>
       </c>
       <c r="H65" s="22"/>

</xml_diff>